<commit_message>
overhauling extract and transform
</commit_message>
<xml_diff>
--- a/data_pipeline/dimensional_data_CSVs/Beaufort_scale.xlsx
+++ b/data_pipeline/dimensional_data_CSVs/Beaufort_scale.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tofad\weather_data_pipeline\data_pipeline\dimensional_data_CSVs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ED8A89-1487-4840-905B-803C39269FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,148 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>wind_speed_upper_ms</t>
+  </si>
+  <si>
+    <t>wind_speed_upper_m_s</t>
+  </si>
+  <si>
+    <t>beaufort</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Calm</t>
+  </si>
+  <si>
+    <t>Light air</t>
+  </si>
+  <si>
+    <t>Light breeze</t>
+  </si>
+  <si>
+    <t>Gentle breeze</t>
+  </si>
+  <si>
+    <t>Moderate breeze</t>
+  </si>
+  <si>
+    <t>Fresh breeze</t>
+  </si>
+  <si>
+    <t>Strong breeze</t>
+  </si>
+  <si>
+    <t>Near gale</t>
+  </si>
+  <si>
+    <t>Gale</t>
+  </si>
+  <si>
+    <t>Strong gale</t>
+  </si>
+  <si>
+    <t>Storm</t>
+  </si>
+  <si>
+    <t>Violent storm</t>
+  </si>
+  <si>
+    <t>Hurricane</t>
+  </si>
+  <si>
+    <t>Sea like a mirror</t>
+  </si>
+  <si>
+    <t>Smoke drift indicates wind direction; vanes do not move</t>
+  </si>
+  <si>
+    <t>Ripples with the appearance of scales; no foam crests</t>
+  </si>
+  <si>
+    <t>Wind felt on face; leaves rustle; vanes begin to move</t>
+  </si>
+  <si>
+    <t>Leaves and small twigs in constant motion; light flags extended</t>
+  </si>
+  <si>
+    <t>Large wavelets; crests begin to break; scattered whitecaps</t>
+  </si>
+  <si>
+    <t>Dust and loose paper raised; small branches move</t>
+  </si>
+  <si>
+    <t>Small waves becoming longer; numerous whitecaps</t>
+  </si>
+  <si>
+    <t>Small wavelets; crests glassy; no breaking</t>
+  </si>
+  <si>
+    <t>Small trees in leaf begin to sway</t>
+  </si>
+  <si>
+    <t>Crested wavelets form moderate waves</t>
+  </si>
+  <si>
+    <t>Branches of moderate size move; small trees sway</t>
+  </si>
+  <si>
+    <t>Moderate waves taking more form; many whitecaps; some spray</t>
+  </si>
+  <si>
+    <t>Large branches in motion; whistling in wires; umbrellas difficult to use</t>
+  </si>
+  <si>
+    <t>Large waves developing; foam crests more extensive; spray likely</t>
+  </si>
+  <si>
+    <t>Whole trees in motion; inconvenience walking against wind</t>
+  </si>
+  <si>
+    <t>Moderately high waves with breaking crests; spindrift begins</t>
+  </si>
+  <si>
+    <t>Twigs break off trees; walking generally impeded</t>
+  </si>
+  <si>
+    <t>High waves; dense streaks of foam; spray may reduce visibility</t>
+  </si>
+  <si>
+    <t>Slight structural damage occurs</t>
+  </si>
+  <si>
+    <t>Very high waves; long overhanging crests; foam blown in dense white streaks</t>
+  </si>
+  <si>
+    <t>Trees uprooted; considerable structural damage</t>
+  </si>
+  <si>
+    <t>Exceptionally high waves; sea completely covered with foam and spray; visibility greatly reduced</t>
+  </si>
+  <si>
+    <t>Devastation; widespread damage</t>
+  </si>
+  <si>
+    <t>Air filled with foam and spray; sea completely white; visibility near zero</t>
+  </si>
+  <si>
+    <t>land_conditions</t>
+  </si>
+  <si>
+    <t>sea_conditions</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +476,304 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="58.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="80.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>0.3</v>
+      </c>
+      <c r="D3">
+        <v>1.5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>1.6</v>
+      </c>
+      <c r="D4">
+        <v>3.3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>3.4</v>
+      </c>
+      <c r="D5">
+        <v>5.4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>5.5</v>
+      </c>
+      <c r="D6">
+        <v>7.9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>10.7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>10.8</v>
+      </c>
+      <c r="D8">
+        <v>13.8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>13.9</v>
+      </c>
+      <c r="D9">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>17.2</v>
+      </c>
+      <c r="D10">
+        <v>20.7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>20.8</v>
+      </c>
+      <c r="D11">
+        <v>24.4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>24.5</v>
+      </c>
+      <c r="D12">
+        <v>28.4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>28.5</v>
+      </c>
+      <c r="D13">
+        <v>32.6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>